<commit_message>
fix various typos and added section labels in the abstracts
</commit_message>
<xml_diff>
--- a/BESETO Presentations.xlsx
+++ b/BESETO Presentations.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="212">
   <si>
     <t>Type</t>
   </si>
@@ -105,9 +105,6 @@
     <t xml:space="preserve">The Attitude and Perception of Physicians on Early Diagnosis and Treatment of Alzheimer’s Disease: A Nationwide Cross-sectional Survey (APPEAL) in China </t>
   </si>
   <si>
-    <t>Recent senior since relationship. Really accept mean surface each. Democrat team treat last least shake. Product happy fine represent last turn sometimes. Road hard situation go adult. Standard key its chance military style become. Save sure common drop call. Site low low school. Attorney company thank sea myself star need. Conference happy physical be audience economy land. Skill specific degree suddenly great. Morning factor account near church. Majority they step hand. This recently piece traditional let million activity.</t>
-  </si>
-  <si>
     <t>Moonyoung Yang</t>
   </si>
   <si>
@@ -117,7 +114,10 @@
     <t>Altered cortical gyrification as a predictive marker of treatment resistance in patients with first-episode psychosis</t>
   </si>
   <si>
-    <t>Objective Predicting resistance to usual treatment from the beginning of psychotic disorder is important for improving prognosis, however, biomarkers to predict treatment resistance in early psychosis have not yet been sufficiently investigated. Thus, we investigated whether patients with first-episode psychosis (FEP) who later were classified as treatment-resistant (TRs) and not as treatment-resistant (non-TRs) have different cortical gyrification patterns compared to healthy controls (HCs). Methods A total of 101 FEP patients and 101 matched HCs underwent T1-weighted magnetic resonance imaging. FEP patients were provided antipsychotic medication during their follow-up period. TR was defined when a patient was taking clozapine or showing moderate to severe symptoms were present despite of taking more than 2 types of antipsychotics in sufficient amounts and duration at their last follow-up point. The mean follow-up duration was 67 months. Cortical gyrification was calculated using local gyrification index (lGI) in a vertexwise fashion across the entire cortical surface and compared across the TRs, non-TRs, and HCs. Results TRs exhibited significant reduction in cortical gyrification compared to HCs in clusters including precuneus, cuneus, and lingual gyri. Meanwhile, non-TRs exhibited significantly reduced cortical gyrification than HCs in clusters including precentral and postcentral areas. Conclusion Our findings of different gyrification patterns between TRs and non-TRs suggest that different neurodevelopment abnormalities may underlie TRs and non-TRs. These results suggest that cortical gyrification could be a biomarker for predicting treatment resistance to usual antipsychotic medication from the beginning of psychotic disorders which may aid treatment strategies to TRs to improve their prognosis.</t>
+    <t>**Objective** Predicting resistance to usual treatment from the beginning of psychotic disorder is important for improving prognosis, however, biomarkers to predict treatment resistance in early psychosis have not yet been sufficiently investigated. Thus, we investigated whether patients with first-episode psychosis (FEP) who later were classified as treatment-resistant (TRs) and not as treatment-resistant (non-TRs) have different cortical gyrification patterns compared to healthy controls (HCs).
+**Methods** A total of 101 FEP patients and 101 matched HCs underwent T1-weighted magnetic resonance imaging. FEP patients were provided antipsychotic medication during their follow-up period. TR was defined when a patient was taking clozapine or showing moderate to severe symptoms were present despite of taking more than 2 types of antipsychotics in sufficient amounts and duration at their last follow-up point. The mean follow-up duration was 67 months. Cortical gyrification was calculated using local gyrification index (lGI) in a vertexwise fashion across the entire cortical surface and compared across the TRs, non-TRs, and HCs.
+**Results** TRs exhibited significant reduction in cortical gyrification compared to HCs in clusters including precuneus, cuneus, and lingual gyri. Meanwhile, non-TRs exhibited significantly reduced cortical gyrification than HCs in clusters including precentral and postcentral areas.
+**Conclusion** Our findings of different gyrification patterns between TRs and non-TRs suggest that different neurodevelopment abnormalities may underlie TRs and non-TRs. These results suggest that cortical gyrification could be a biomarker for predicting treatment resistance to usual antipsychotic medication from the beginning of psychotic disorders which may aid treatment strategies to TRs to improve their prognosis.</t>
   </si>
   <si>
     <t xml:space="preserve">Masashi Mizutani </t>
@@ -147,16 +147,13 @@
     <t>1,20</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Therapeutic outcomes wide association scan (TOWAS) of different antipsychotics in schizophrenia
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Background: We aimed to identify discrepant therapeutic outcomes among different antipsychotics in a RCT. 
-Methods: A total of 3030 patients with schizophrenia from a RCT were enrolled as discovery cohort, and 1395 patients as validation cohorts. TOWAS was conducted to scan differentiate outcomes of 209 therapeutic outcomes across antipsychotics. 
-Outcomes: Olanzapine significantly related to higher risk of AIWG, liver dysfunction, sedation, increased lipid, and lower risk of EPS. Risperidone related to higher risk of HPRL. Quetiapine related to higher risk of sedation, palpitation, increased lipid, lower risk of HPRL, and EPS. Aripiprazole related to lower risk of HPRL, AIWG, sedation, and QTc prolongation. Ziprasidone related to higher risk of increased QT, nausea, lower risk of AIWG, liver dysfunction, and increased lipid. Haloperidol related to higher risk of EPS, HPRL, and increased salivation. Perphenazine related to higher risk of EPS. 
-Conclusion: Further independent RCT-designed cohort is necessary for validation.
-</t>
+    <t>Therapeutic outcomes wide association scan (TOWAS) of different antipsychotics in schizophrenia</t>
+  </si>
+  <si>
+    <t>**Background:** We aimed to identify discrepant therapeutic outcomes among different antipsychotics in a RCT.
+**Methods:** A total of 3030 patients with schizophrenia from a RCT were enrolled as discovery cohort, and 1395 patients as validation cohorts. TOWAS was conducted to scan differentiate outcomes of 209 therapeutic outcomes across antipsychotics. 
+**Outcomes:** Olanzapine significantly related to higher risk of AIWG, liver dysfunction, sedation, increased lipid, and lower risk of EPS. Risperidone related to higher risk of HPRL. Quetiapine related to higher risk of sedation, palpitation, increased lipid, lower risk of HPRL, and EPS. Aripiprazole related to lower risk of HPRL, AIWG, sedation, and QTc prolongation. Ziprasidone related to higher risk of increased QT, nausea, lower risk of AIWG, liver dysfunction, and increased lipid. Haloperidol related to higher risk of EPS, HPRL, and increased salivation. Perphenazine related to higher risk of EPS.
+**Conclusion:** Further independent RCT-designed cohort is necessary for validation.</t>
   </si>
   <si>
     <t>pptx</t>
@@ -168,14 +165,13 @@
     <t xml:space="preserve">Increased neuromelanin accumulation in schizophrenia patients: a neuromelanin-sensitive MRI study        </t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: To examine the neuromelanin (NM) levels of schizophrenia and to determine whether the levels are related to symptom scores
-Methods: We acquired NM-MRI data from 30 schizophrenia patients (average age 25.50; % male 50) and 64 age- and sex-matched healthy controls (24.25; 46.88). We calculated the contrast ratio by placing a circular mask on the substantia nigra (SN) and crus cerebri. The contrast ratio was compared between groups, and correlation with symptomatic scores was investigated in schizophrenia patients.
-Results: In schizophrenia, the contrast ratio of the SN was increased compared to the healthy controls (p = 0.042, Cohen's d = 0.425). There was no correlation between the contrast ratio and symptom score in schizophrenia patients. 
-Conclusion: These results are in line with previous studies reporting increased NM and excessive dopamine production in the SN. This study proposes the possibility of using NM changes as a biomarker for schizophrenia. 
-</t>
-  </si>
-  <si>
-    <t>Yukata Sawai</t>
+    <t>**Objective:** To examine the neuromelanin (NM) levels of schizophrenia and to determine whether the levels are related to symptom scores
+**Methods:** We acquired NM-MRI data from 30 schizophrenia patients (average age 25.50; % male 50) and 64 age- and sex-matched healthy controls (24.25; 46.88). We calculated the contrast ratio by placing a circular mask on the substantia nigra (SN) and crus cerebri. The contrast ratio was compared between groups, and correlation with symptomatic scores was investigated in schizophrenia patients.
+**Results:** In schizophrenia, the contrast ratio of the SN was increased compared to the healthy controls (p = 0.042, Cohen's d = 0.425). There was no correlation between the contrast ratio and symptom score in schizophrenia patients. 
+**Conclusion:** These results are in line with previous studies reporting increased NM and excessive dopamine production in the SN. This study proposes the possibility of using NM changes as a biomarker for schizophrenia.</t>
+  </si>
+  <si>
+    <t>Yutaka Sawai</t>
   </si>
   <si>
     <t>1,24,39</t>
@@ -214,10 +210,10 @@
     <t>Verbal fluency data as a predictor of clinical course of individuals at clinical high-risk for psychosis</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective This study aims to investigate whether verbal fluency task measure other than word count could be a predictor of prognosis, especially remission, of individuals at clinical high risk (CHR) for psychosis.
-Methods 127 CHR individuals and 178 healthy controls underwent verbal fluency task. Semantic clusters in individual task response were extracted, using Korean word embedding model. Word count, average cluster size, and maximum cluster size were put into binomial logistic regression model to verify if each of the variables predict conversion or remission of CHRs.
-Results Logistic regression analysis revealed that word count of verbal fluency task response could only predict conversion at baseline. For non-converters, average and maximum size of semantic clusters were able to significantly distinguish remitters from non-remitters.
-Conclusion This study suggests that verbal fluency task measures that are more related to semantic organization than word count could be a predictor of remission of CHR individuals.
+    <t xml:space="preserve">**Objective** This study aims to investigate whether verbal fluency task measure other than word count could be a predictor of prognosis, especially remission, of individuals at clinical high risk (CHR) for psychosis.
+**Methods** 127 CHR individuals and 178 healthy controls underwent verbal fluency task. Semantic clusters in individual task response were extracted, using Korean word embedding model. Word count, average cluster size, and maximum cluster size were put into binomial logistic regression model to verify if each of the variables predict conversion or remission of CHRs.
+**Results** Logistic regression analysis revealed that word count of verbal fluency task response could only predict conversion at baseline. For non-converters, average and maximum size of semantic clusters were able to significantly distinguish remitters from non-remitters.
+**Conclusion** This study suggests that verbal fluency task measures that are more related to semantic organization than word count could be a predictor of remission of CHR individuals.
 </t>
   </si>
   <si>
@@ -242,7 +238,11 @@
     <t>Clinical Characteristics of Comorbid Tic Disorders in Autism Spectrum Disorder-Exploratory Analysis</t>
   </si>
   <si>
-    <t>MISSING ABSTRACT</t>
+    <t xml:space="preserve">**Objective** To investigate the prevalence of comorbid tic disorders in individuals with ASD using standardized assessment methods. Secondly, to explore differences in ASD symptom severity and other comorbidities.
+**Methods** We included individuals diagnosed with ASD (n = 679) aged 4 to 18 years who completed the YGTSS questionnaire. Based on the YGTSS score, the included individuals were divided into two groups: ASD only (n = 554) and ASD with tics (n = 125).
+**Results** The ASD with tics group had a significantly higher average age and full-scale IQ score than the ASD only group. Regarding clinical characteristics, the ASD with tics group showed significantly higher SRS-2, CBCL, and YBOCS subdomain scores after adjusting for age. Individuals with a higher IQ (IQ ≥70) showed a significantly greater proportion of tic symptoms.
+**Conclusions** The severity of ASD core and comorbid symptoms is associated with tic disorders and severity among affected individuals.
+</t>
   </si>
   <si>
     <t>Favour Omileke</t>
@@ -267,10 +267,10 @@
     <t>Incongruent grey matter atrophy and functional connectivity of striatal subregions in behavioral variant frontotemporal dementia</t>
   </si>
   <si>
-    <t>Objective: To explore the structure and function of striatal subregions in bvFTD.
-Methods: We acquired T1 and fMRI data from 26 bvFTD patients and 36 control subjects. We used VBM and RSFC analyses to study group differences in striatal subregions. Correlation analyses were used to investigate the relationship between imaging and neuropsychological tests.
-Results: The patients of bvFTD had smaller volumes of striatal subregions than the controls. And we found that the ventral atrophy was greater than dorsal atrophy, and the right greater than the left. Functional imaging analysis revealed that bvFTD patients exhibited different changed patterns in striatal subregions compared to controls, and the RSFC extending range on the right was greater than that on the left in the same subregions. The dorsolateral putamen nucleus was involved in executive function regulation.
-Conclusion: This suggests that incongruent structural and functional changes in striatal subregions may underly the bvFTD cognitive deficit.</t>
+    <t>**Objective:** To explore the structure and function of striatal subregions in bvFTD.
+**Methods:** We acquired T1 and fMRI data from 26 bvFTD patients and 36 control subjects. We used VBM and RSFC analyses to study group differences in striatal subregions. Correlation analyses were used to investigate the relationship between imaging and neuropsychological tests.
+**Results:** The patients of bvFTD had smaller volumes of striatal subregions than the controls. And we found that the ventral atrophy was greater than dorsal atrophy, and the right greater than the left. Functional imaging analysis revealed that bvFTD patients exhibited different changed patterns in striatal subregions compared to controls, and the RSFC extending range on the right was greater than that on the left in the same subregions. The dorsolateral putamen nucleus was involved in executive function regulation.
+**Conclusion:** This suggests that incongruent structural and functional changes in striatal subregions may underly the bvFTD cognitive deficit.</t>
   </si>
   <si>
     <t>Inkyung Park</t>
@@ -279,10 +279,10 @@
     <t>Cortical gyrification differences between early- and late-onset obsessive–compulsive disorder: Neurobiological evidence for neurodevelopmentally distinct subtypes</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective. Identifying neurodevelopmental differences in subtypes of patients with obsessive–compulsive disorder (OCD) is critical for understanding complexities of the disorder and establishing biological evidence-based homogeneous subtypes in this heterogeneous population.
-Methods. We compared whole-brain cortical gyrification in 84 patients with early-onset OCD, 84 patients with late-onset OCD, and 152 healthy controls using the local gyrification index (lGI). Then, the relationships between lGI in clusters showing significant differences and performance of trait-related neurocognitive function impairments in OCD was further examined in early-onset OCD patients.
-Results. The early-onset OCD patients exhibited significantly greater gyrification than those with late-onset OCD patients and healthy controls in frontoparietal and cingulate regions. Moreover, impaired neurocognitive functions in early-onset OCD patients were correlated with increased gyrification.
-Conclusion. Our findings provide a neurobiological marker to distinguish the OCD population into more neurodevelopmentally homogeneous subtypes, which may contribute to the understanding of the neurodevelopmental underpinnings of an etiology. 
+    <t xml:space="preserve">**Objective.** Identifying neurodevelopmental differences in subtypes of patients with obsessive–compulsive disorder (OCD) is critical for understanding complexities of the disorder and establishing biological evidence-based homogeneous subtypes in this heterogeneous population.
+**Methods.** We compared whole-brain cortical gyrification in 84 patients with early-onset OCD, 84 patients with late-onset OCD, and 152 healthy controls using the local gyrification index (lGI). Then, the relationships between lGI in clusters showing significant differences and performance of trait-related neurocognitive function impairments in OCD was further examined in early-onset OCD patients.
+**Results.** The early-onset OCD patients exhibited significantly greater gyrification than those with late-onset OCD patients and healthy controls in frontoparietal and cingulate regions. Moreover, impaired neurocognitive functions in early-onset OCD patients were correlated with increased gyrification.
+**Conclusion.** Our findings provide a neurobiological marker to distinguish the OCD population into more neurodevelopmentally homogeneous subtypes, which may contribute to the understanding of the neurodevelopmental underpinnings of an etiology. 
 </t>
   </si>
   <si>
@@ -295,8 +295,7 @@
     <t xml:space="preserve">Group-exercise participation, executive function and associated brain structures in children with ADHD </t>
   </si>
   <si>
-    <t xml:space="preserve">The current research aimed to explore if frequent participation in group-based exercise can predict better executive function performance in children with attention-deficit/hyperactivity disorder (ADHD). Furthermore, we aimed to explore whether this relationship is mediated by white matter regions associated with the cerebellum (ROI). 30 typically developing (TD) children and 46 children with ADHD participated in the current study. A two-way ANCOVA revealed an interaction effect that approached significance (p=0.057). A further t-test revealed that those who frequently participated in group exercise performed significantly better in executive function than those who didn’t, only in the ADHD group.  Analysis involving the ROI revealed that medial lemniscus (left) (β=0.09**, p=0.004) and pontine crossing tract (left) (β=0.07*, p=0.036) volumes have a significant mediating effect on the executive function performance. The results revealed that the effects of frequent participation in group-based exercise on executive functioning was mediated by several regions associated with the cerebellum.
-</t>
+    <t>The current research aimed to explore if frequent participation in group-based exercise can predict better executive function performance in children with attention-deficit/hyperactivity disorder (ADHD). Furthermore, we aimed to explore whether this relationship is mediated by white matter regions associated with the cerebellum (ROI). 30 typically developing (TD) children and 46 children with ADHD participated in the current study. A two-way ANCOVA revealed an interaction effect that approached significance (p=0.057). A further t-test revealed that those who frequently participated in group exercise performed significantly better in executive function than those who didn’t, only in the ADHD group.  Analysis involving the ROI revealed that medial lemniscus (left) (β=0.09\*\*, p=0.004) and pontine crossing tract (left) (β=0.07\*, p=0.036) volumes have a significant mediating effect on the executive function performance. The results revealed that the effects of frequent participation in group-based exercise on executive functioning was mediated by several regions associated with the cerebellum.</t>
   </si>
   <si>
     <t>Yankun Wu</t>
@@ -318,10 +317,10 @@
     <t>Frontoparietal White Matter Anatomy in Patients with Obsessive-Compulsive Disorder</t>
   </si>
   <si>
-    <t>Objective: Despite functional dysconnectivity and altered white matter (WM) integrity of frontoparietal regions, the anatomical profile of the superior longitudinal fasciculus (SLF) remains unclear in the complex pathophysiology of obsessive-compulsive disorder. Thus, we aimed to examine the WM integrity of SLF I, II, and III in patients with OCD.  
-Methods: 90 unmedicated OCD patients and 81 healthy controls (HCs) were scanned with diffusion weighted imaging. We conducted whole-brain tractography and virtual dissections of SLF subdivisions. Averaged diffusion measures were extracted from each SLF subdivision and compared between groups.
-Results: No significant difference was found in all diffusion measures of SLF subdivisions between the OCD patients and HCs.
-Conclusion: We indicate no substantial change in WM integrity of frontoparietal connections in OCD patients. Given the large sample size and reliable method, we suggest that rather the aberrant WM projections, altered cortical function in frontoparietal regions may primarily underlie the OCD pathophysiology.</t>
+    <t>**Objective:** Despite functional dysconnectivity and altered white matter (WM) integrity of frontoparietal regions, the anatomical profile of the superior longitudinal fasciculus (SLF) remains unclear in the complex pathophysiology of obsessive-compulsive disorder. Thus, we aimed to examine the WM integrity of SLF I, II, and III in patients with OCD.  
+**Methods:** 90 unmedicated OCD patients and 81 healthy controls (HCs) were scanned with diffusion weighted imaging. We conducted whole-brain tractography and virtual dissections of SLF subdivisions. Averaged diffusion measures were extracted from each SLF subdivision and compared between groups.
+**Results:** No significant difference was found in all diffusion measures of SLF subdivisions between the OCD patients and HCs.
+**Conclusion:** We indicate no substantial change in WM integrity of frontoparietal connections in OCD patients. Given the large sample size and reliable method, we suggest that rather the aberrant WM projections, altered cortical function in frontoparietal regions may primarily underlie the OCD pathophysiology.</t>
   </si>
   <si>
     <t>Eimu Shoji</t>
@@ -396,10 +395,10 @@
     <t>Characteristics of primary age-related tauopathy defined by neuroimaging biomarkers</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: Primary age-related tauopathy (PART) is a neuropathological entity with neurofibrillary tangles (NFTs) in the absence of beta-amyloid (Aβ) plaques in the brain. We tried to investigate the frequency and rate of cognitive decline in older adults with PART defined by neuroimaging biomarkers.
-Methods: A total of 161 older individuals were included in the analysis. PART was defined when SUVR value of mean global Aβ deposition is less than 1.4 (Aβ negative) and tau burden corresponds to Braak stage I-IV. 
-Results: Among 161 participants, 51 (31.7%) were classified as PART, 31 (19.3 %) as no Alzheimer's disease (AD)-pathology, and 79 (49.1%) as AD. In regard to cognitive change rate, PART was similar to no-AD pathology with a relatively stable course which was significantly slower than AD. 
-Conclusion: Our findings indicate that PART is relatively common in older adults and PART appears closer to no-AD pathology condition rather than AD.
+    <t xml:space="preserve">**Objective:** Primary age-related tauopathy (PART) is a neuropathological entity with neurofibrillary tangles (NFTs) in the absence of beta-amyloid (Aβ) plaques in the brain. We tried to investigate the frequency and rate of cognitive decline in older adults with PART defined by neuroimaging biomarkers.
+**Methods:** A total of 161 older individuals were included in the analysis. PART was defined when SUVR value of mean global Aβ deposition is less than 1.4 (Aβ negative) and tau burden corresponds to Braak stage I-IV. 
+**Results:** Among 161 participants, 51 (31.7%) were classified as PART, 31 (19.3 %) as no Alzheimer's disease (AD)-pathology, and 79 (49.1%) as AD. In regard to cognitive change rate, PART was similar to no-AD pathology with a relatively stable course which was significantly slower than AD. 
+**Conclusion:** Our findings indicate that PART is relatively common in older adults and PART appears closer to no-AD pathology condition rather than AD.
 </t>
   </si>
   <si>
@@ -440,10 +439,10 @@
     <t>Mental Health Concerns in Parents of Children with Autism Spectrum Disorder</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: This study aims to explore the mental health of parents whose child has been diagnosed with autism spectrum disorder (ASD).  
-Methods: Mental health problems were assessed using the Korean-Symptom Check List 95 (K-SCL95), a self-report questionnaire that screens for 20 mental health conditions. Parents were divided into two groups depending on the presence of mental health problems. Independent t-tests and ANCOVA were used to explore the clinical characteristics between the groups. 
-Results: A total of 186 parents (120 with and 86 without mental health problems) of children with ASD were included. The group with mental health problems scored higher in self-rating scales of social communication, rigid personality, and pragmatic language difficulties (p-values &lt; .001~.011). No significant differences in the child’s ASD-related symptoms were found between the groups. 
-Conclusion: Parents of children with ASD also require support to address difficulties with mental health.  </t>
+    <t xml:space="preserve">**Objective:** This study aims to explore the mental health of parents whose child has been diagnosed with autism spectrum disorder (ASD).  
+**Methods:** Mental health problems were assessed using the Korean-Symptom Check List 95 (K-SCL95), a self-report questionnaire that screens for 20 mental health conditions. Parents were divided into two groups depending on the presence of mental health problems. Independent t-tests and ANCOVA were used to explore the clinical characteristics between the groups. 
+**Results:** A total of 186 parents (120 with and 86 without mental health problems) of children with ASD were included. The group with mental health problems scored higher in self-rating scales of social communication, rigid personality, and pragmatic language difficulties (p-values &lt; .001~.011). No significant differences in the child’s ASD-related symptoms were found between the groups. 
+**Conclusion:** Parents of children with ASD also require support to address difficulties with mental health.  </t>
   </si>
   <si>
     <t>Kaori Usui</t>
@@ -478,16 +477,22 @@
     <t>Different executive function impairments in medication-naïve children with attention-deficit/hyperactivity disorder comorbid with oppositional defiant disorder and conduct disorder</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction: Disruptive behavior disorders (DBD), including oppositional defiant disorder (ODD) and conduct disorder (CD), is the most common comorbidity in ADHD. Few studies have separated ADHD with CD (ADHDCD+) and ADHD with ODD (ADHDODD+) when studying the executive functions (EFs) and brain imaging of ADHD with DBD (ADHDDBD+).
-Methods: EFs difference were compared in 1,026 ADHDDBD+ (104 ADHDCD+, 922 ADHDODD+), 1,026 ADHDonly and 406 healthy controls (HCs). Brain activation of 164 children with ADHD were also measured to investigate the neural basis with functional near-infrared spectroscopy (fNIRS),
-Results: No EFs impairment was seen between ADHDCD+ and HCs. More severe CD symptoms were associated with better EFs. The relationship between CD symptoms and inhibition function was mediated by the FC of SMN(L) - DMN(R).
-Conclusion: ADHDCD+ and ADHDODD+ showed difference in EFs impairment. The comorbid of CD may not worsen the impairments, even be with better EFs performance within ADHD individuals. 
+    <t xml:space="preserve">**Introduction:** Disruptive behavior disorders (DBD), including oppositional defiant disorder (ODD) and conduct disorder (CD), is the most common comorbidity in ADHD. Few studies have separated ADHD with CD (ADHDCD+) and ADHD with ODD (ADHDODD+) when studying the executive functions (EFs) and brain imaging of ADHD with DBD (ADHDDBD+).
+**Methods:** EFs difference were compared in 1,026 ADHDDBD+ (104 ADHDCD+, 922 ADHDODD+), 1,026 ADHDonly and 406 healthy controls (HCs). Brain activation of 164 children with ADHD were also measured to investigate the neural basis with functional near-infrared spectroscopy (fNIRS).
+**Results:** No EFs impairment was seen between ADHDCD+ and HCs. More severe CD symptoms were associated with better EFs. The relationship between CD symptoms and inhibition function was mediated by the FC of SMN(L) - DMN(R).
+**Conclusion:** ADHDCD+ and ADHDODD+ showed difference in EFs impairment. The comorbid of CD may not worsen the impairments, even be with better EFs performance within ADHD individuals. 
 </t>
   </si>
   <si>
     <t>Jinju Jung</t>
   </si>
   <si>
+    <t xml:space="preserve">Auditory verbal hallucinations (AVH) are a core positive symptom of schizophrenia and are regarded as a consequence of the functional breakdown in the related sensory process. Yet, the potential mechanism of AVH is still lacking. 
+In the present study, we explored the difference between AVHs (n = 23) and non-AVHs (n = 19) in schizophrenia and healthy controls (n = 29) by using multidimensional electroencephalograms data during an auditory oddball task. Comparing to healthy controls, both AVH and non-AVH groups showed reduced P300 amplitudes. Even more, brain networks analysis results found AVH patients showed reduced left frontal to posterior parietal/temporal connectivity than non-AVH patients. Moreover, when using the fused network properties of both delta and theta bands as features for in-depth learning, it was possible to identify the AVH from non-AVH patients at an accuracy of 80.95%. 
+The left frontal-parietal/temporal networks seen in the auditory oddball paradigm might be underlying biomarkers of AVH in schizophrenia. This study demonstrated for the first time the functional breakdown of the auditory processing pathway in the AVH patients, leading to a better understanding of the atypical brain network of the AVH. 
+</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
@@ -497,10 +502,10 @@
     <t>A 15-year follow-up study of dementia</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: To define the frailty definition, describe incidence and its distribution, and to explore risk factors.
-Methods: A 15-year follow-up study was conducted in 2022 participants aged 65 years and over in Beijing, China. Three evaluation criteria of frailty were constructed. The incidence of dementia was calculated, and the risk factors of dementia were analyzed. 
-Results: The 15-year cumulative incidence of dementia was 14.94%, the incidence density was 25.02/1000 person-years. The behavioral and psychological symptoms (RR=2.247, 95% CI:1.500-3.151), depression (RR=2.110, 95% CI: 1.365-3.038), frailty defined by physical frailty index (PFI) (RR=1.514, 95% CI:1.123-1.997) and frailty defined by multidimensional frailty index (MFI) (RR=1.669, 95% CI:1.312-2.059) were risk factors of dementia, fish consumption was a protective factor of dementia (RR=0.749,95% CI:0.574-0.970).
-Conclusion: Depression, behavioral and psychological symptoms, frailty defined by PFI and MFI increase the risk of dementia, and regular consumption of fish reduce the risk of dementia. 
+    <t xml:space="preserve">**Objective:** To define the frailty definition, describe incidence and its distribution, and to explore risk factors.
+**Methods:** A 15-year follow-up study was conducted in 2022 participants aged 65 years and over in Beijing, China. Three evaluation criteria of frailty were constructed. The incidence of dementia was calculated, and the risk factors of dementia were analyzed. 
+**Results:** The 15-year cumulative incidence of dementia was 14.94%, the incidence density was 25.02/1000 person-years. The behavioral and psychological symptoms (RR=2.247, 95% CI:1.500-3.151), depression (RR=2.110, 95% CI: 1.365-3.038), frailty defined by physical frailty index (PFI) (RR=1.514, 95% CI:1.123-1.997) and frailty defined by multidimensional frailty index (MFI) (RR=1.669, 95% CI:1.312-2.059) were risk factors of dementia, fish consumption was a protective factor of dementia (RR=0.749,95% CI:0.574-0.970).
+**Conclusion:** Depression, behavioral and psychological symptoms, frailty defined by PFI and MFI increase the risk of dementia, and regular consumption of fish reduce the risk of dementia. 
 </t>
   </si>
   <si>
@@ -513,9 +518,9 @@
     <t>Development and validation of cerebral white matter hyperintensity probability map of Korean elderly</t>
   </si>
   <si>
-    <t xml:space="preserve">Background and Purpose: Although previously constructed white matter hyperintensity (WMH) probability maps of healthy older adults exist, they have several limitations in representing the distribution of WMH in healthy older adults, especially Asian older adults. We developed and validated a WMH probability map (WPM) of healthy older Koreans and examined the age-associated differences of WMH. 
-Methods: We constructed WPM using development dataset that consisted of high-resolution 3D fluid-attenuated inversion recovery images of 5 age groups (60–64 years, 65–69 years, 70–74 years, 75–79 years, and 80+ years). Each age group included 30 age-matched men and women each. We tested the validity of the WPM by comparing WMH ages estimated by the WPM and the chronological ages of 30 healthy controls, 30 hypertension patients, and 30 stroke patients. 
-Results: Older age groups showed a higher volume of WMH in both hemispheres (p &lt; 0.001). About 90% of the WMH were located in periventricular space in all age groups. With advancing age, the peak of the distance histogram from the ventricular wall of the periventricular WMH shifted away from the ventricular wall, while that of deep WMH shifted toward the ventricular wall. The estimated WMH ages were comparable to the chronological ages in the healthy controls, while being higher than the chronological ages in hypertension and stroke patients. 
+    <t xml:space="preserve">**Background and Purpose:** Although previously constructed white matter hyperintensity (WMH) probability maps of healthy older adults exist, they have several limitations in representing the distribution of WMH in healthy older adults, especially Asian older adults. We developed and validated a WMH probability map (WPM) of healthy older Koreans and examined the age-associated differences of WMH. 
+**Methods:** We constructed WPM using development dataset that consisted of high-resolution 3D fluid-attenuated inversion recovery images of 5 age groups (60–64 years, 65–69 years, 70–74 years, 75–79 years, and 80+ years). Each age group included 30 age-matched men and women each. We tested the validity of the WPM by comparing WMH ages estimated by the WPM and the chronological ages of 30 healthy controls, 30 hypertension patients, and 30 stroke patients. 
+**Results:** Older age groups showed a higher volume of WMH in both hemispheres (p &lt; 0.001). About 90% of the WMH were located in periventricular space in all age groups. With advancing age, the peak of the distance histogram from the ventricular wall of the periventricular WMH shifted away from the ventricular wall, while that of deep WMH shifted toward the ventricular wall. The estimated WMH ages were comparable to the chronological ages in the healthy controls, while being higher than the chronological ages in hypertension and stroke patients. 
 </t>
   </si>
   <si>
@@ -575,10 +580,10 @@
     <t>Synergistic interaction of high blood pressure and cerebral beta-amyloid on tau pathology</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: To understand the link between hypertension and Alzheimer disease, this cross-sectional study examined the relationships of hypertension history and current blood pressure (BP) with in vivo β-amyloid (Aβ) and tau deposition, and whether hypertension history and current BP modulate the relationship between Aβ and tau.
-Methods: All 68 cognitively normal older adults underwent both Aβ and tau positron emission tomography, as well as clinical assessment of hypertension history and current BP.
-Results: Using linear regression models, neither the history nor current BP had direct association with Aβ or tau. However, the synergistic interaction effects of high current systolic and diastolic BP with Aβ on tau were significant, whereas there was no such effect for history of hypertension.
-Conclusion: High current BP, but not hypertension history, modulate the relationship between cerebral Aβ and tau deposition in late-life, and thus strict BP control is warranted in cognitively normal older adults with hypertension.
+    <t xml:space="preserve">**Objective:** To understand the link between hypertension and Alzheimer disease, this cross-sectional study examined the relationships of hypertension history and current blood pressure (BP) with in vivo β-amyloid (Aβ) and tau deposition, and whether hypertension history and current BP modulate the relationship between Aβ and tau.
+**Methods:** All 68 cognitively normal older adults underwent both Aβ and tau positron emission tomography, as well as clinical assessment of hypertension history and current BP.
+**Results:** Using linear regression models, neither the history nor current BP had direct association with Aβ or tau. However, the synergistic interaction effects of high current systolic and diastolic BP with Aβ on tau were significant, whereas there was no such effect for history of hypertension.
+**Conclusion:** High current BP, but not hypertension history, modulate the relationship between cerebral Aβ and tau deposition in late-life, and thus strict BP control is warranted in cognitively normal older adults with hypertension.
 </t>
   </si>
   <si>
@@ -601,8 +606,7 @@
     <t>23,35</t>
   </si>
   <si>
-    <t xml:space="preserve">Analysis of the relationship between activated plasma MMP9 levels and volumes of subcortical regions.
-</t>
+    <t>Analysis of the relationship between activated plasma MMP9 levels and volumes of subcortical regions</t>
   </si>
   <si>
     <t xml:space="preserve">Matrix metalloproteinase 9 (MMP9) is an enzyme involved in the degradation of the extracellular matrix in human physiological processes. MMP9 is expressed in some brain regions including hippocampus, and it influences learning and memory processes. Recently, it has been reported that plasma MMP9 levels in schizophrenia were significantly higher than in healthy controls, and they were negatively correlated with bilateral hippocampal volumes. However, the associations of activated plasma MMP9 levels and volumes of subcortical regions including hippocampus remains elusive. Thus, we investigated whether activated plasma MMP9 levels are associated with volumes of subcortical regions including hippocampus and using blood samples and T1-weighted MRI images of 28 patients with schizophrenia and 50 healthy controls. MRI images were analyzed with FreeSurfer software. Activated plasma MMP9 levels were negatively associated with volumes of right hippocampus in the schizophrenia group, while they were not associated with volumes of any subcortical region in healthy controls. These results suggest that activated MMP9 may break down the brain extracellular matrix, leading to brain volume reduction of right hippocampus in schizophrenia.
@@ -618,8 +622,7 @@
     <t>24,39</t>
   </si>
   <si>
-    <t xml:space="preserve">The longitudinal relationship between dissociative symptoms and self-harm in adolescents: A population-based cohort study.
-</t>
+    <t>The longitudinal relationship between dissociative symptoms and self-harm in adolescents: A population-based cohort study</t>
   </si>
   <si>
     <t xml:space="preserve">Previous cross-sectional studies have reported that dissociative symptoms (DIS) are associated with self-harm (SH). We aimed to investigate the longitudinal relationship between DIS and SH in general adolescent population. 
@@ -635,14 +638,14 @@
     <t>Analyses of REM sleep without atonia and neurocognitive function in REM sleep behavior disorder</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: We aimed to determine the relationship between REM sleep without atonia (RSWA) and neurocognitive function among patients with idiopathic REM sleep behavior disorder (iRBD). 
-Methods: We retrospectively analyzed the baseline polysomnographic recordings and neurocognitive data of 45 Korean iRBD patients. The quantitative analysis of electromyography during REM sleep was performed by manual method, according to the American Academy of Sleep Medicine (AASM) manual for scoring sleep, 2007. Neurocognitive data included both quantitative electroencephalography (qEEG) and neuropsychological measures. 
-Results: Patients with high phasic RSWA showed poorer performance in digit span forward (p=0.008), increased absolute delta power in temporal (p=0.045) and parietal (p=0.035) regions, and increased absolute theta power in parietal (p=0.035) regions. However, patients with high tonic RSWA got lower scores only in trail-making test B (p=0.009). Also, phasic RSWA was significantly correlated with absolute delta and theta power, categorical fluency, and mini-mental state examination (MMSE-KC). Regarding tonic RSWA, there was no significant correlation other than Boston naming test. 
-Conclusion: This study suggests that phasic rather than tonic RSWA reflects changes in the underlying neurocognitive function of iRBD patients.
-</t>
-  </si>
-  <si>
-    <t>Mashiro Kiyota</t>
+    <t xml:space="preserve">**Objective:** We aimed to determine the relationship between REM sleep without atonia (RSWA) and neurocognitive function among patients with idiopathic REM sleep behavior disorder (iRBD). 
+**Methods:** We retrospectively analyzed the baseline polysomnographic recordings and neurocognitive data of 45 Korean iRBD patients. The quantitative analysis of electromyography during REM sleep was performed by manual method, according to the American Academy of Sleep Medicine (AASM) manual for scoring sleep, 2007. Neurocognitive data included both quantitative electroencephalography (qEEG) and neuropsychological measures. 
+**Results:** Patients with high phasic RSWA showed poorer performance in digit span forward (p=0.008), increased absolute delta power in temporal (p=0.045) and parietal (p=0.035) regions, and increased absolute theta power in parietal (p=0.035) regions. However, patients with high tonic RSWA got lower scores only in trail-making test B (p=0.009). Also, phasic RSWA was significantly correlated with absolute delta and theta power, categorical fluency, and mini-mental state examination (MMSE-KC). Regarding tonic RSWA, there was no significant correlation other than Boston naming test. 
+**Conclusion:** This study suggests that phasic rather than tonic RSWA reflects changes in the underlying neurocognitive function of iRBD patients.
+</t>
+  </si>
+  <si>
+    <t>Masahiro Kiyota</t>
   </si>
   <si>
     <t>The associations of behavioral/emotional problems with testosterone and amygdala volume in early adolescent boys</t>
@@ -657,10 +660,10 @@
     <t>Comparison of Autonomous sensory meridian response and binaural auditory beats effects on stress reduction: A randomized double-blind trial</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective: This study aimed to compare the effects of Autonomous sensory meridian response (ASMR) and binaural beat (BB) on stress reduction.
-Method: Subjects with stress were recruited considering their perceived stress scale (PSS), Beck depression inventory-II (BDI-II), insomnia severity index (ISI), and state-trait anxiety inventory-state anxiety (STAI-S) scores. Subjects listened to ASMR or BB with music (8Hz, 15minutes for daytime, 5Hz, 30 minutes for nighttime) for 3 weeks. QEEG was measured before and after the intervention.
-Results: Seventy-six participants finished the trial. After the intervention, PSS, BDI-II, ISI, STAI-S, and PSQI scores improved significantly in both groups. Changes of absolute beta and high beta power in the ASMR group were larger than those in the BB group (p = 0.026, p = 0.040, respectively). 
-Conclusion: ASMR and BB are equally effective in reducing stress. ASMR can lead to an increase in beta and high beta waves associated with cortical arousal.
+    <t xml:space="preserve">**Objective:** This study aimed to compare the effects of Autonomous sensory meridian response (ASMR) and binaural beat (BB) on stress reduction.
+**Method:** Subjects with stress were recruited considering their perceived stress scale (PSS), Beck depression inventory-II (BDI-II), insomnia severity index (ISI), and state-trait anxiety inventory-state anxiety (STAI-S) scores. Subjects listened to ASMR or BB with music (8Hz, 15minutes for daytime, 5Hz, 30 minutes for nighttime) for 3 weeks. QEEG was measured before and after the intervention.
+**Results:** Seventy-six participants finished the trial. After the intervention, PSS, BDI-II, ISI, STAI-S, and PSQI scores improved significantly in both groups. Changes of absolute beta and high beta power in the ASMR group were larger than those in the BB group (p = 0.026, p = 0.040, respectively). 
+**Conclusion:** ASMR and BB are equally effective in reducing stress. ASMR can lead to an increase in beta and high beta waves associated with cortical arousal.
 </t>
   </si>
   <si>
@@ -670,11 +673,11 @@
     <t>Development of a computer application to predict suicidal attempt: A prospective cohort study</t>
   </si>
   <si>
-    <t xml:space="preserve">Objectives: We established a prediction model for suicide-attempts, validated it in an independent cohort, and developed a computerized prediction program. 
-Methods: For suicidal ideators and attempters in Korean COhort Model Predicting Suicide and Suicidal-behavior(K-COMPASS) during 2015.11~2019.7, we performed logistic regression for suicide-attempts within 6months. We validated this model in an independent cohort during 2019.8~2022.6. Meanwhile, another model was constructed using self-report scales to develop a risk prediction application without professional assessment.
-Results: Among 800 participants, 452 followed-up until 6 months, and 32 attempted suicide. Accuracy was AUC=0.824, PPV=17.67%, sensitivity=0.723 and specificity=0.841. Meanwhile, among 432 in validation cohort, 128 followed-up and 6 attempted suicides by 6months. Accuracy of our model in the validation cohort was AUC=0.771, sensitivity = 1.00 and specificity=0.578.
+    <t xml:space="preserve">**Objectives:** We established a prediction model for suicide-attempts, validated it in an independent cohort, and developed a computerized prediction program. 
+**Methods:** For suicidal ideators and attempters in Korean COhort Model Predicting Suicide and Suicidal-behavior(K-COMPASS) during 2015.11~2019.7, we performed logistic regression for suicide-attempts within 6months. We validated this model in an independent cohort during 2019.8~2022.6. Meanwhile, another model was constructed using self-report scales to develop a risk prediction application without professional assessment.
+**Results:** Among 800 participants, 452 followed-up until 6 months, and 32 attempted suicide. Accuracy was AUC=0.824, PPV=17.67%, sensitivity=0.723 and specificity=0.841. Meanwhile, among 432 in validation cohort, 128 followed-up and 6 attempted suicides by 6months. Accuracy of our model in the validation cohort was AUC=0.771, sensitivity = 1.00 and specificity=0.578.
 Accuracy of self-report model was AUC=0.834, PPV=9.69%, sensitivity=0.894 and specificity=0.698 in the original cohort; AUC=0.725, sensitivity=0.571, and specificity=0.532 in validation cohort.
-Conclusion: Our program could be widely used in mental-healthcare blind-spots such as military or prison.
+**Conclusion:** Our program could be widely used in mental-healthcare blind-spots such as military or prison.
 </t>
   </si>
   <si>
@@ -684,10 +687,10 @@
     <t>An epidemiological study of mental disability in community adults in China</t>
   </si>
   <si>
-    <t>Objective: To describe the epidemic strength of mental disability, and explore its risk factors.
-Methods: Based on the data of China Mental Health Survey, prevalence of disability of mental disorders and disability rate among patients were calculated, risk factors of mental disability were analyzed by multivariate logistic regression.
-Results: Prevalence of disability of any mental disorder among mood disorder, anxiety disorder, substance-use disorder, intermittent explosive disorder, and eating disorder was 2.84%, disability rate among patients was 31.95%. Risk factors of mental disability were people aged 80 and over (OR=8.98), comorbid other mental disorders and physical diseases (OR=6.50), people aged 65 to 79 (OR=3.00), having received psychiatric treatment in the past 12 months (OR=2.46), comorbid physical diseases (OR=2.00).
-Conclusion: People aged 65 and over, comorbid mental disorders and physical diseases, having received psychiatric treatment in the past 12 months are high-risk populations of mental disability in the Chinese community.</t>
+    <t>**Objective:** To describe the epidemic strength of mental disability, and explore its risk factors.
+**Methods:** Based on the data of China Mental Health Survey, prevalence of disability of mental disorders and disability rate among patients were calculated, risk factors of mental disability were analyzed by multivariate logistic regression.
+**Results:** Prevalence of disability of any mental disorder among mood disorder, anxiety disorder, substance-use disorder, intermittent explosive disorder, and eating disorder was 2.84%, disability rate among patients was 31.95%. Risk factors of mental disability were people aged 80 and over (OR=8.98), comorbid other mental disorders and physical diseases (OR=6.50), people aged 65 to 79 (OR=3.00), having received psychiatric treatment in the past 12 months (OR=2.46), comorbid physical diseases (OR=2.00).
+**Conclusion:** People aged 65 and over, comorbid mental disorders and physical diseases, having received psychiatric treatment in the past 12 months are high-risk populations of mental disability in the Chinese community.</t>
   </si>
   <si>
     <t>Changhyeon Baek</t>
@@ -699,10 +702,10 @@
     <t>Influence of biogenetic explanations of mental disorders on stigma and help seeking behavior A systematic review and meta analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">Objectives: Biogenetic causal explanations of mental disorders are commonly used for public education and campaigns. However, the influence of biogenetic explanations on the ideas about and attitudes toward mental illness is unclear. We examined the influence of biogenetic explanations on attitudes toward mental disorders using a meta-analytic method accompanied by subgroup analyses. 
-Methods: Experimental and correlational studies were analyzed separately. Five outcome measures related to attitudes toward mental disorders were included: ‘attitude toward help-seeking’, ‘blame’, ‘perceived dangerousness’, ‘prognostic pessimism’, and ‘social distance’. Subgroup analyses were performed for the type of mental disorder, population, and geographic region for which a biogenetic explanation was provided.
-Results: A total of 44 studies were included, of which 24 were experimental and 20 were correlational. A positive attitude toward help-seeking was associated with having a biogenetic concept (d = 0.43, P &lt; 0.001) in general population and in Eastern countries in particular. Although a biogenetic explanation was associated with a decreased level of blame (d = −0.20, P = 0.03) in the general population, it was also associated with significantly higher levels of perceived dangerousness (d = 0.13, 95% CI 0.03 to 0.23, P = 0.008). A tendency toward a higher level of prognostic pessimism and social distance was associated with a biogenetic concept of mental disorders although there was no statistical significance. 
-Conclusions: Although a biogenetic explanation promotes public use of mental health services, it should be carefully applied to avoid an increase in negative thoughts, such as that mental illness is biologically irreversible and untreatable.
+    <t xml:space="preserve">**Objectives:** Biogenetic causal explanations of mental disorders are commonly used for public education and campaigns. However, the influence of biogenetic explanations on the ideas about and attitudes toward mental illness is unclear. We examined the influence of biogenetic explanations on attitudes toward mental disorders using a meta-analytic method accompanied by subgroup analyses. 
+**Methods:** Experimental and correlational studies were analyzed separately. Five outcome measures related to attitudes toward mental disorders were included: ‘attitude toward help-seeking’, ‘blame’, ‘perceived dangerousness’, ‘prognostic pessimism’, and ‘social distance’. Subgroup analyses were performed for the type of mental disorder, population, and geographic region for which a biogenetic explanation was provided.
+**Results:** A total of 44 studies were included, of which 24 were experimental and 20 were correlational. A positive attitude toward help-seeking was associated with having a biogenetic concept (d = 0.43, P &lt; 0.001) in general population and in Eastern countries in particular. Although a biogenetic explanation was associated with a decreased level of blame (d = −0.20, P = 0.03) in the general population, it was also associated with significantly higher levels of perceived dangerousness (d = 0.13, 95% CI 0.03 to 0.23, P = 0.008). A tendency toward a higher level of prognostic pessimism and social distance was associated with a biogenetic concept of mental disorders although there was no statistical significance. 
+**Conclusions:** Although a biogenetic explanation promotes public use of mental health services, it should be carefully applied to avoid an increase in negative thoughts, such as that mental illness is biologically irreversible and untreatable.
 </t>
   </si>
   <si>
@@ -712,10 +715,10 @@
     <t>Systematic Review of Cognitive Behavioral Therapy Programs on GamingInternet Use Disorder Focusing on CBT Techniques Used</t>
   </si>
   <si>
-    <t xml:space="preserve">Object: This study thus aimed to review the contents and CBT techniques used in previously reported CBT programs for IA/IGD. 
-Method: A database search of Ovid/MEDLINE, EMBASE, Cochran, CINAHL, PsychINFO, WOS was conducted for IA/IGD CBT interventions. A total of 4860 articles were identified, and 22 articles were included in the study criteria. CBT techniques used in programs were identified and categorized by two separate psychiatrists. 
-Results: Programs varied in length, from 4 to 24 sessions. The time spent on each session also varied from 40 to 120 minutes. Among techniques used in CBT, problem solving skill training was the most widely used, and cognitive reconstruction was the second most widely used. Time spent in behavioral therapy was longer than that in cognitive therapy in general. 
-Conclusion: CBT programs for IA/IGD varied in session length and included CBT techniques. Programs were usually more focused on behavioral therapy. Theory and evidence-based standardization of IA/IGD CBT programs is required. 
+    <t xml:space="preserve">**Object:** This study thus aimed to review the contents and CBT techniques used in previously reported CBT programs for IA/IGD. 
+**Method:** A database search of Ovid/MEDLINE, EMBASE, Cochran, CINAHL, PsychINFO, WOS was conducted for IA/IGD CBT interventions. A total of 4860 articles were identified, and 22 articles were included in the study criteria. CBT techniques used in programs were identified and categorized by two separate psychiatrists. 
+**Results:** Programs varied in length, from 4 to 24 sessions. The time spent on each session also varied from 40 to 120 minutes. Among techniques used in CBT, problem solving skill training was the most widely used, and cognitive reconstruction was the second most widely used. Time spent in behavioral therapy was longer than that in cognitive therapy in general. 
+**Conclusion:** CBT programs for IA/IGD varied in session length and included CBT techniques. Programs were usually more focused on behavioral therapy. Theory and evidence-based standardization of IA/IGD CBT programs is required. 
 </t>
   </si>
   <si>
@@ -741,7 +744,10 @@
     <t>Prevalence of Depressive Disorders and Treatment in China: A Cross-sectional Study</t>
   </si>
   <si>
-    <t>Objective: To describe the epidemic strength of mental disability, and explore its risk factors. Methods: Based on the data of China Mental Health Survey, prevalence of disability of mental disorders and disability rate among patients were calculated, risk factors of mental disability were analyzed by multivariate logistic regression. Results: Prevalence of disability of any mental disorder among mood disorder, anxiety disorder, substance-use disorder, intermittent explosive disorder, and eating disorder was 2.84%, disability rate among patients was 31.95%. Risk factors of mental disability were people aged 80 and over (OR=8.98), comorbid other mental disorders and physical diseases (OR=6.50), people aged 65 to 79 (OR=3.00), having received psychiatric treatment in the past 12 months (OR=2.46), comorbid physical diseases (OR=2.00). Conclusion: People aged 65 and over, comorbid mental disorders and physical diseases, having received psychiatric treatment in the past 12 months are high-risk populations of mental disability in Chinese community.</t>
+    <t>**Objective:** To describe the epidemic strength of mental disability, and explore its risk factors. 
+**Methods:** Based on the data of China Mental Health Survey, prevalence of disability of mental disorders and disability rate among patients were calculated, risk factors of mental disability were analyzed by multivariate logistic regression.
+**Results:** Prevalence of disability of any mental disorder among mood disorder, anxiety disorder, substance-use disorder, intermittent explosive disorder, and eating disorder was 2.84%, disability rate among patients was 31.95%. Risk factors of mental disability were people aged 80 and over (OR=8.98), comorbid other mental disorders and physical diseases (OR=6.50), people aged 65 to 79 (OR=3.00), having received psychiatric treatment in the past 12 months (OR=2.46), comorbid physical diseases (OR=2.00).
+**Conclusion:** People aged 65 and over, comorbid mental disorders and physical diseases, having received psychiatric treatment in the past 12 months are high-risk populations of mental disability in Chinese community.</t>
   </si>
   <si>
     <t>Jae-Hyun Han</t>
@@ -753,9 +759,11 @@
     <t>Prenatal and Perinatal risk factors for Autism spectrum disorder</t>
   </si>
   <si>
-    <t>Objective: Although ASD seems to be under the influence of a strong genetic etiology, the concordance rate of identical twins is reported to be around 60%, and since the concordance rate is not 100%, environmental factors can also be considered. The purpose of this study was to evaluate the prenatal and perinatal history of children with autism spectrum disorder (ASD) as compared to unaffected siblings (SIB). Methods: Subjects with ASD and their SIB were recruited. All subjects were assessed using both the Korean version of Autism Diagnostic Interview-Revised (K-ADI-R) and the Korean version of Autism Diagnostic Observation Schedule (K-ADOS) and were subsequently identified as affected or unaffected. Prenatal and perinatal  history was obtained from the primary caregivers and each facet was compared in those with ASD and the SIB groups using SPSS ver. 25.0 (p&lt;.05).
-Results: 875 individuals with ASD (143 females, 87.87±42.35months), 244 SIB (135 females, 91.52±32.01 months) were analyzed. The ASD group showed significantly higher rates of neonatal jaundice (χ2=6.620, p=.010, OR=1.721), insufficient MMR vaccination (χ2=11.532, p=.001, OR=1.808) and tic symptoms (χ2=13.086, p=.000, OR=5.38). Differences in the frequency of seizure, birth trauma, respiratory distress and motor dysfunction at birth were not significantly different among the two groups.
-Conclusion: These results indicate that perinatal and prenatal factors may contribute to the development of ASD. The results imply that rather than being a single cause, environmental factors are also important in the ASD group or suggest the presence of gene-environment interactions. Large-scale prospective studies are needed.</t>
+    <t xml:space="preserve">**Objective:** Although ASD seems to be under the influence of a strong genetic etiology, the concordance rate of identical twins is reported to be around 60%, and since the concordance rate is not 100%, environmental factors can also be considered. The purpose of this study was to evaluate the prenatal and perinatal history of children with autism spectrum disorder (ASD) as compared to unaffected siblings (SIB).
+**Methods:** Subjects with ASD and their SIB were recruited. All subjects were assessed using both the Korean version of Autism Diagnostic Interview-Revised (K-ADI-R) and the Korean version of Autism Diagnostic Observation Schedule (K-ADOS) and were subsequently identified as affected or unaffected. Prenatal and perinatal  history was obtained from the primary caregivers and each facet was compared in those with ASD and the SIB groups using SPSS ver. 25.0 (p&lt;.05).
+**Results:** 875 individuals with ASD (143 females, 87.87±42.35months), 244 SIB (135 females, 91.52±32.01 months) were analyzed. The ASD group showed significantly higher rates of neonatal jaundice (χ2=6.620, p=.010, OR=1.721), insufficient MMR vaccination (χ2=11.532, p=.001, OR=1.808) and tic symptoms (χ2=13.086, p=.000, OR=5.38). Differences in the frequency of seizure, birth trauma, respiratory distress and motor dysfunction at birth were not significantly different among the two groups.
+**Conclusion:** These results indicate that perinatal and prenatal factors may contribute to the development of ASD. The results imply that rather than being a single cause, environmental factors are also important in the ASD group or suggest the presence of gene-environment interactions. Large-scale prospective studies are needed.
+</t>
   </si>
   <si>
     <t>Shuntaro Ando</t>
@@ -764,9 +772,11 @@
     <t>Tokyo Teen Cohort Study: A Prospective Cohort Study on General Population of Adolescents</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction: Adolescence is the period when many mental disorders have their peaks of onsets. Objectives: This study aimed to prospectively reveal the developmental trajectory of physical and mental health in adolescence, and to investigate factors associated with the trajectory. Patients/Materials and Methods: We launched a prospective cohort study (Tokyo Teen Cohort: TTC) on general population of adolescents at three municipalities in metropolitan area in Tokyo, Japan. Using the resident register, we recruited 10-year-old children from the community between 2012 and 2015. The second, third, and fourth wave of data collection were conducted at 12, 14, 16 years of age, respectively. We collected multidisciplinary data including mental health by self-report questionnaire and home-visit interview. Further, we have launched two subsample studies which focus on biological measures such as brain MRI, EEG, and sex hormones. TTC is based at three research institutes, and ethics approval has been granted by all of the three institutions.
-Results: A total of 3171 children participated the TTC. Of those, 3007 children participated in the second wave of data collection (follow-up rate: 94.8%). The third and fourth wave of data collection were completed and more than 80% of children continued to participate in TTC. More than 300 children participated in the two subsample studies. More than 30 papers were already published, and many national/international research collaborations have started. Conclusion: The fifth wave of data collection at 20 years of age is being currently conducted. Further national/international collaborations are expected to examine cultural effects on mental health of adolescents.
-</t>
+    <t>**Introduction:** Adolescence is the period when many mental disorders have their peaks of onsets. 
+**Objectives:** This study aimed to prospectively reveal the developmental trajectory of physical and mental health in adolescence, and to investigate factors associated with the trajectory.
+**Patients/Materials and Methods:** We launched a prospective cohort study (Tokyo Teen Cohort: TTC) on general population of adolescents at three municipalities in metropolitan area in Tokyo, Japan. Using the resident register, we recruited 10-year-old children from the community between 2012 and 2015. The second, third, and fourth wave of data collection were conducted at 12, 14, 16 years of age, respectively. We collected multidisciplinary data including mental health by self-report questionnaire and home-visit interview. Further, we have launched two subsample studies which focus on biological measures such as brain MRI, EEG, and sex hormones. TTC is based at three research institutes, and ethics approval has been granted by all of the three institutions.
+**Results:** A total of 3171 children participated the TTC. Of those, 3007 children participated in the second wave of data collection (follow-up rate: 94.8%). The third and fourth wave of data collection were completed and more than 80% of children continued to participate in TTC. More than 300 children participated in the two subsample studies. More than 30 papers were already published, and many national/international research collaborations have started.
+**Conclusion:** The fifth wave of data collection at 20 years of age is being currently conducted. Further national/international collaborations are expected to examine cultural effects on mental health of adolescents.</t>
   </si>
 </sst>
 </file>
@@ -841,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -878,9 +888,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1282,9 +1289,7 @@
       <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="J5" s="11"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6">
@@ -1305,16 +1310,16 @@
         <v>17</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="K6" s="5"/>
     </row>
@@ -1336,25 +1341,25 @@
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="J7" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="K7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C8" s="1">
         <v>1.0</v>
@@ -1369,27 +1374,27 @@
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="J8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C9" s="1">
         <v>2.0</v>
@@ -1404,27 +1409,27 @@
         <v>17</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H9" s="3">
         <v>1.0</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C10" s="1">
         <v>3.0</v>
@@ -1439,27 +1444,27 @@
         <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C11" s="1">
         <v>4.0</v>
@@ -1474,27 +1479,27 @@
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>5.0</v>
@@ -1509,27 +1514,27 @@
         <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C13" s="1">
         <v>7.0</v>
@@ -1544,27 +1549,27 @@
         <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C14" s="1">
         <v>8.0</v>
@@ -1578,28 +1583,28 @@
       <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>65</v>
+      <c r="G14" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="H14" s="3">
         <v>10.0</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>67</v>
-      </c>
       <c r="K14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C15" s="1">
         <v>9.0</v>
@@ -1614,27 +1619,27 @@
         <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>70</v>
-      </c>
       <c r="K15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1">
         <v>1.0</v>
@@ -1649,27 +1654,27 @@
         <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>75</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1">
         <v>2.0</v>
@@ -1684,27 +1689,27 @@
         <v>17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H17" s="3">
         <v>35.0</v>
       </c>
       <c r="I17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="1">
         <v>3.0</v>
@@ -1719,27 +1724,27 @@
         <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>82</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="1">
         <v>4.0</v>
@@ -1754,27 +1759,27 @@
         <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="J19" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="11" t="s">
-        <v>86</v>
-      </c>
       <c r="K19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1">
         <v>5.0</v>
@@ -1789,27 +1794,27 @@
         <v>17</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H20" s="3">
         <v>35.0</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="K20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1">
         <v>6.0</v>
@@ -1824,27 +1829,27 @@
         <v>22</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H21" s="3">
         <v>35.0</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>92</v>
-      </c>
       <c r="K21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="1">
         <v>7.0</v>
@@ -1859,27 +1864,27 @@
         <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="K22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1">
         <v>8.0</v>
@@ -1894,27 +1899,27 @@
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="J23" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="K23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1">
         <v>9.0</v>
@@ -1929,27 +1934,27 @@
         <v>12</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J24" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="K24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C25" s="1">
         <v>1.0</v>
@@ -1963,28 +1968,28 @@
       <c r="F25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="J25" s="11" t="s">
-        <v>109</v>
-      </c>
       <c r="K25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="1">
         <v>2.0</v>
@@ -1999,27 +2004,27 @@
         <v>17</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H26" s="3">
         <v>6.0</v>
       </c>
       <c r="I26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>112</v>
-      </c>
       <c r="K26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1">
         <v>3.0</v>
@@ -2034,27 +2039,27 @@
         <v>22</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="J27" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="J27" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="K27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" s="1">
         <v>4.0</v>
@@ -2069,27 +2074,27 @@
         <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H28" s="3">
         <v>20.0</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="K28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C29" s="1">
         <v>5.0</v>
@@ -2104,27 +2109,27 @@
         <v>17</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H29" s="3">
         <v>10.0</v>
       </c>
       <c r="I29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J29" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="J29" s="11" t="s">
-        <v>122</v>
-      </c>
       <c r="K29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" s="1">
         <v>6.0</v>
@@ -2139,27 +2144,27 @@
         <v>22</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="J30" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="J30" s="11" t="s">
-        <v>126</v>
-      </c>
       <c r="K30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" s="1">
         <v>7.0</v>
@@ -2174,27 +2179,27 @@
         <v>12</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="J31" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="J31" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="K31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="1">
         <v>8.0</v>
@@ -2209,27 +2214,27 @@
         <v>12</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H32" s="3">
         <v>10.0</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="J32" s="11" t="s">
-        <v>133</v>
-      </c>
       <c r="K32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" s="1">
         <v>9.0</v>
@@ -2244,24 +2249,24 @@
         <v>12</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J33" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="K33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>135</v>
@@ -2278,7 +2283,7 @@
       <c r="F34" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="13" t="s">
         <v>136</v>
       </c>
       <c r="H34" s="3">
@@ -2291,12 +2296,12 @@
         <v>138</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>135</v>
@@ -2326,12 +2331,12 @@
         <v>142</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>135</v>
@@ -2361,12 +2366,12 @@
         <v>146</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>135</v>
@@ -2396,12 +2401,12 @@
         <v>149</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>135</v>
@@ -2431,12 +2436,12 @@
         <v>153</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>135</v>
@@ -2466,12 +2471,12 @@
         <v>157</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>135</v>
@@ -2494,19 +2499,19 @@
       <c r="H40" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="13" t="s">
         <v>160</v>
       </c>
       <c r="J40" s="11" t="s">
         <v>161</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>135</v>
@@ -2536,12 +2541,12 @@
         <v>165</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>135</v>
@@ -2556,7 +2561,7 @@
         <v>0.6041666666666666</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>166</v>
@@ -2571,12 +2576,12 @@
         <v>169</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>170</v>
@@ -2606,12 +2611,12 @@
         <v>174</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>170</v>
@@ -2641,12 +2646,12 @@
         <v>177</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>170</v>
@@ -2667,7 +2672,7 @@
         <v>178</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>179</v>
@@ -2676,12 +2681,12 @@
         <v>180</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>170</v>
@@ -2711,12 +2716,12 @@
         <v>183</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>170</v>
@@ -2746,12 +2751,12 @@
         <v>186</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>170</v>
@@ -2781,12 +2786,12 @@
         <v>189</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>170</v>
@@ -2809,19 +2814,19 @@
       <c r="H49" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="I49" s="14" t="s">
+      <c r="I49" s="13" t="s">
         <v>192</v>
       </c>
       <c r="J49" s="11" t="s">
         <v>193</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>170</v>
@@ -2851,7 +2856,7 @@
         <v>196</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51">
@@ -2875,7 +2880,7 @@
         <v>198</v>
       </c>
       <c r="H51" s="3"/>
-      <c r="I51" s="15" t="s">
+      <c r="I51" s="14" t="s">
         <v>199</v>
       </c>
       <c r="J51" s="11" t="s">
@@ -2965,7 +2970,7 @@
       <c r="G54" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H54" s="15">
         <v>10.0</v>
       </c>
       <c r="I54" s="12" t="s">
@@ -2977,13 +2982,13 @@
       <c r="K54" s="5"/>
     </row>
     <row r="55">
-      <c r="J55" s="17"/>
+      <c r="J55" s="16"/>
     </row>
     <row r="56">
-      <c r="J56" s="18"/>
+      <c r="J56" s="17"/>
     </row>
     <row r="57">
-      <c r="J57" s="19"/>
+      <c r="J57" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$K$57"/>
@@ -2991,7 +2996,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B54">
       <formula1>"A,B,C,D,E"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="H2:H9 H10:I10 H11:H54">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="H2:H54">
       <formula1>REGEXMATCH(TO_TEXT(H2), "^[0-9,]+$")</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="数値を入力してください 次の値以上 1" sqref="C2:C54">

</xml_diff>